<commit_message>
Added todo list and udpates to calendar
</commit_message>
<xml_diff>
--- a/calendar/Calendar.xlsx
+++ b/calendar/Calendar.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gabehope/Documents/Courses/cs152.github.io/calendar/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gabehope/Documents/Documents - Mac/Courses/cs152.github.io/calendar/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33DDB6E5-557F-924A-9BD9-79630B3F3876}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4437C25-00A1-FD4D-8F6C-A8977BC788F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1160" windowWidth="30240" windowHeight="17360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="900" windowWidth="30240" windowHeight="17360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="154">
   <si>
     <t>Week</t>
   </si>
@@ -325,6 +325,54 @@
     <t xml:space="preserve">Linear regression, maximum likelihood </t>
   </si>
   <si>
+    <t>Lecture 3</t>
+  </si>
+  <si>
+    <r>
+      <t>Homework 2 assigned ([</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>Drive</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF3B3B3B"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>](</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="12"/>
+        <color rgb="FF3B3B3B"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>https://drive.google.com/drive/folders/1deohwJarw4aa-Te3DYDrdbn35v1EWIsm?usp=drive_link</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF3B3B3B"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>Logistic regression</t>
+  </si>
+  <si>
     <r>
       <t>[</t>
     </r>
@@ -335,6 +383,147 @@
         <rFont val="Menlo"/>
         <family val="2"/>
       </rPr>
+      <t>Book 1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF3B3B3B"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>](</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="12"/>
+        <color rgb="FF3B3B3B"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>https://probml.github.io/pml-book/book1.html</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF3B3B3B"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">): 10.1, 10.2.1, 10.2.3, 10.3.1-10.3.3 </t>
+    </r>
+  </si>
+  <si>
+    <t>Lecture 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Multinomial logistic regression </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[Book 1](https://probml.github.io/pml-book/book1.html): 10.2.2 </t>
+  </si>
+  <si>
+    <t>Feature transforms</t>
+  </si>
+  <si>
+    <r>
+      <t>[</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>Book 1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF3B3B3B"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>](</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="12"/>
+        <color rgb="FF3B3B3B"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>https://probml.github.io/pml-book/book1.html</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF3B3B3B"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>): 13.1, 13.2</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Neural networks </t>
+  </si>
+  <si>
+    <r>
+      <t>[</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>Book 1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF3B3B3B"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>](</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="12"/>
+        <color rgb="FF3B3B3B"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>https://probml.github.io/pml-book/book1.html</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF3B3B3B"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">): 13.1, 13.2 </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>[</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
       <t>Notes</t>
     </r>
     <r>
@@ -354,6 +543,1131 @@
         <rFont val="Menlo"/>
         <family val="2"/>
       </rPr>
+      <t>../lecture5-neural-networks-intro/notes.qmd</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF3B3B3B"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">) </t>
+    </r>
+  </si>
+  <si>
+    <t>lecture 7</t>
+  </si>
+  <si>
+    <r>
+      <t>Homework 3 assigned ([</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>Drive</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF3B3B3B"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>](</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="12"/>
+        <color rgb="FF3B3B3B"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>https://drive.google.com/drive/folders/1Df96GdFpucM-YUf6c5PTWUfxWY-UrLXl?usp=drive_link</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF3B3B3B"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>))</t>
+    </r>
+  </si>
+  <si>
+    <t>Deep neural networks</t>
+  </si>
+  <si>
+    <t>Automatic Differentiation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[Book 1](https://probml.github.io/pml-book/book1.html): 13.3 </t>
+  </si>
+  <si>
+    <r>
+      <t>[</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>Notes</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF3B3B3B"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>](</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="12"/>
+        <color rgb="FF3B3B3B"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>../lecture6-backpropagation/notes.qmd</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF3B3B3B"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">) </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Homework 4 assigned ([</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>Drive</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF3B3B3B"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>](</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="12"/>
+        <color rgb="FF3B3B3B"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>https://drive.google.com/drive/folders/1wIblhOu4c0LlbiveKP1Z2uTVre3d62pO?usp=drive_link</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF3B3B3B"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>))</t>
+    </r>
+  </si>
+  <si>
+    <t>Homework 3 Due</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reverse-mode Automatic Differentiation </t>
+  </si>
+  <si>
+    <r>
+      <t>[</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>Book 1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF3B3B3B"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>](</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="12"/>
+        <color rgb="FF3B3B3B"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>https://probml.github.io/pml-book/book1.html</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF3B3B3B"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">): 13.4.5, 13.5 </t>
+    </r>
+  </si>
+  <si>
+    <t>PyTorch</t>
+  </si>
+  <si>
+    <r>
+      <t>[</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>Book 1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF3B3B3B"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>](</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="12"/>
+        <color rgb="FF3B3B3B"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>https://probml.github.io/pml-book/book1.html</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF3B3B3B"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>): 13.5</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve"> [Notebook](https://drive.google.com/file/d/1N76hpENuKchbfN0o-NZ02FAgZYPiWPVf/view?usp=drive_link)</t>
+  </si>
+  <si>
+    <r>
+      <t>Homework 5 assigned ([</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>Drive</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF3B3B3B"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>](</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="12"/>
+        <color rgb="FF3B3B3B"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>https://drive.google.com/drive/folders/1C9vFAnO_sogGupxvOrU4uQl8ZkF7seU5?usp=drive_link</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF3B3B3B"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>))</t>
+    </r>
+  </si>
+  <si>
+    <t>Homework 4 Due</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L1 &amp; L2 regularization </t>
+  </si>
+  <si>
+    <r>
+      <t>[</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>Book 1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF3B3B3B"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>](</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="12"/>
+        <color rgb="FF3B3B3B"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>https://probml.github.io/pml-book/book1.html</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF3B3B3B"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">): 8.4 </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Regularization (Cont.), Dropout </t>
+  </si>
+  <si>
+    <r>
+      <t>[</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>Book 1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF3B3B3B"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>](</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="12"/>
+        <color rgb="FF3B3B3B"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>https://probml.github.io/pml-book/book1.html</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF3B3B3B"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>): 13.4.1-13.4.2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Homework 6 assigned ([</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>Drive</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF3B3B3B"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>](</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="12"/>
+        <color rgb="FF3B3B3B"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>https://drive.google.com/drive/u/1/folders/1ohI5itSgEhBNmKSLQSjwmJlgWjioWDhi</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF3B3B3B"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>))</t>
+    </r>
+  </si>
+  <si>
+    <t>Homework 5 Due</t>
+  </si>
+  <si>
+    <t>Stochastic gradient descent</t>
+  </si>
+  <si>
+    <r>
+      <t>[</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>Book 1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF3B3B3B"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>](</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="12"/>
+        <color rgb="FF3B3B3B"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>https://probml.github.io/pml-book/book1.html</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF3B3B3B"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">): 14.1-14.3 </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>[</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>Notes</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF3B3B3B"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>](</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="12"/>
+        <color rgb="FF3B3B3B"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>../lecture9-optimization/notes.qmd</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF3B3B3B"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">) </t>
+    </r>
+  </si>
+  <si>
+    <t>Homework 6 Due</t>
+  </si>
+  <si>
+    <t>Spring break</t>
+  </si>
+  <si>
+    <t>Project Proposal Due</t>
+  </si>
+  <si>
+    <t>Residual networks and Normalization</t>
+  </si>
+  <si>
+    <t>Residual networks and Normalization (cont.)</t>
+  </si>
+  <si>
+    <r>
+      <t>[</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>Book 1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF3B3B3B"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>](</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="12"/>
+        <color rgb="FF3B3B3B"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>https://probml.github.io/pml-book/book1.html</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF3B3B3B"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">): 15.1, 15.2.1-15.2.3 </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>[</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>Slides</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF3B3B3B"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>](</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="12"/>
+        <color rgb="FF3B3B3B"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>./notes/lecture14.pdf</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF3B3B3B"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">) </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>[</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>Slides</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF3B3B3B"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>](</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="12"/>
+        <color rgb="FF3B3B3B"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>./notes/lecture15.pdf</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF3B3B3B"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">) </t>
+    </r>
+  </si>
+  <si>
+    <t>Convolutional Networks</t>
+  </si>
+  <si>
+    <t>Convolutional Networks (cont.)</t>
+  </si>
+  <si>
+    <r>
+      <t>[</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>Slides</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF3B3B3B"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>](</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="12"/>
+        <color rgb="FF3B3B3B"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>./notes/lecture16.pdf</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF3B3B3B"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">) </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>[</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>Book 1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF3B3B3B"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>](</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="12"/>
+        <color rgb="FF3B3B3B"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>https://probml.github.io/pml-book/book1.html</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF3B3B3B"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">): 15.2.5-15.2.7 </t>
+    </r>
+  </si>
+  <si>
+    <t>Language models, RNNs</t>
+  </si>
+  <si>
+    <r>
+      <t>Homework 7 assigned ([</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>Drive</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF3B3B3B"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>](</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="12"/>
+        <color rgb="FF3B3B3B"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>https://drive.google.com/drive/folders/1vZYEOfmDCfGxWMAAXeEwgMlvCOfKUgle?usp=drive_link</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF3B3B3B"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>))</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Homework 8 assigned ([</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>Drive</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF3B3B3B"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>](</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="12"/>
+        <color rgb="FF3B3B3B"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>https://drive.google.com/drive/folders/1lO11Br_irrOckxZVZdi72MSjR8lTvQ_O?usp=drive_link</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF3B3B3B"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>))</t>
+    </r>
+  </si>
+  <si>
+    <t>[Book 1](https://probml.github.io/pml-book/book1.html): 15.2.1-15.2.6</t>
+  </si>
+  <si>
+    <r>
+      <t>[</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>Slides</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF3B3B3B"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>](</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="12"/>
+        <color rgb="FF3B3B3B"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>./notes/lecture17.pdf</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF3B3B3B"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">) </t>
+    </r>
+  </si>
+  <si>
+    <t>Autoencoders &amp; U-Nets</t>
+  </si>
+  <si>
+    <t>Image models</t>
+  </si>
+  <si>
+    <t>Homework 7 Due</t>
+  </si>
+  <si>
+    <t>Homework 9 assigned</t>
+  </si>
+  <si>
+    <t>Homework 8 Due</t>
+  </si>
+  <si>
+    <r>
+      <t>[</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>Book 1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF3B3B3B"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>](</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="12"/>
+        <color rgb="FF3B3B3B"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>https://probml.github.io/pml-book/book1.html</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF3B3B3B"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>): 15.2.1-15.2.6</t>
+    </r>
+  </si>
+  <si>
+    <t>Attention layers</t>
+  </si>
+  <si>
+    <t>Homework 10 assigned</t>
+  </si>
+  <si>
+    <t>Project check-in assigned</t>
+  </si>
+  <si>
+    <t>Homework 9 Due</t>
+  </si>
+  <si>
+    <t>Transformers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transformers (cont.), Large language models </t>
+  </si>
+  <si>
+    <t>Lecture 25</t>
+  </si>
+  <si>
+    <t>Project check-in due</t>
+  </si>
+  <si>
+    <t>Addressing bias in machine learning</t>
+  </si>
+  <si>
+    <t>Impacts of machine learning</t>
+  </si>
+  <si>
+    <t>Homework 10 Due</t>
+  </si>
+  <si>
+    <t>[Assignment](../assignments/homeworks/homeworks.qmd#Homework-1)</t>
+  </si>
+  <si>
+    <t>[Assignment](../assignments/homeworks/homeworks.qmd#Homework-2)</t>
+  </si>
+  <si>
+    <t>[Assignment](../assignments/homeworks/homeworks.qmd#Homework-3)</t>
+  </si>
+  <si>
+    <t>[Assignment](../assignments/homeworks/homeworks.qmd#Homework-4)</t>
+  </si>
+  <si>
+    <t>[Assignment](../assignments/homeworks/homeworks.qmd#Homework-5)</t>
+  </si>
+  <si>
+    <t>[Assignment](../assignments/homeworks/homeworks.qmd#Homework-6)</t>
+  </si>
+  <si>
+    <t>[Assignment](../assignments/homeworks/homeworks.qmd#Homework-7)</t>
+  </si>
+  <si>
+    <t>[Assignment](../assignments/homeworks/homeworks.qmd#Homework-8)</t>
+  </si>
+  <si>
+    <t>[Assignment](../assignments/homeworks/homeworks.qmd#Homework-9)</t>
+  </si>
+  <si>
+    <t>[Assignment](../assignments/homeworks/homeworks.qmd#Homework-10)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Final project ethics warm-up assigned </t>
+  </si>
+  <si>
+    <t>Ethics Warm-up Due</t>
+  </si>
+  <si>
+    <t>[Assignment](../assignments/final-project/ethics.qmd)</t>
+  </si>
+  <si>
+    <t>[Assignment](../assignments/final-project/outline.qmd)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[Prerequisites](../lecture1-background/prereqs.qmd) [Notes](../lecture1-background/notes.qmd) [slides](../lecture1-background/slides.pdf) </t>
+  </si>
+  <si>
+    <r>
+      <t>[</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>Notes</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF3B3B3B"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>](</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="12"/>
+        <color rgb="FF3B3B3B"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>../lecture8-regularization/notes.qmd</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF3B3B3B"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>[</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>Notes</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF3B3B3B"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>](</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="12"/>
+        <color rgb="FF3B3B3B"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>../lecture8-regularization/notes.qmd</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF3B3B3B"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">) </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>[</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>Notes</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF3B3B3B"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>](</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="12"/>
+        <color rgb="FF3B3B3B"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
       <t>../lecture2-linear-regression/notes.qmd</t>
     </r>
     <r>
@@ -363,15 +1677,15 @@
         <rFont val="Menlo"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">) </t>
-    </r>
-  </si>
-  <si>
-    <t>Lecture 3</t>
-  </si>
-  <si>
-    <r>
-      <t>Homework 2 assigned ([</t>
+      <t>)  [Slides](../lecture2-linear-regression/filled-slides-pt2.pdf)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">[Notes](../lecture2-linear-regression/notes.qmd)  [Slides](../lecture2-linear-regression/filled-slides-pt1.pdf)  [Blank](../lecture2-linear-regression/slides.pdf) </t>
+  </si>
+  <si>
+    <r>
+      <t>[</t>
     </r>
     <r>
       <rPr>
@@ -380,7 +1694,7 @@
         <rFont val="Menlo"/>
         <family val="2"/>
       </rPr>
-      <t>Drive</t>
+      <t>Notes</t>
     </r>
     <r>
       <rPr>
@@ -399,20 +1713,17 @@
         <rFont val="Menlo"/>
         <family val="2"/>
       </rPr>
-      <t>https://drive.google.com/drive/folders/1deohwJarw4aa-Te3DYDrdbn35v1EWIsm?usp=drive_link</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF3B3B3B"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>)</t>
-    </r>
-  </si>
-  <si>
-    <t>Logistic regression</t>
+      <t>../lecture3-logistic-regression/notes.qmd</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF3B3B3B"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>)  [Slides](../lecture3-logistic-regression/filled-slides-pt1.qmd)  [Blank](../lecture3-logistic-regression/slides.qmd)</t>
+    </r>
   </si>
   <si>
     <r>
@@ -425,7 +1736,7 @@
         <rFont val="Menlo"/>
         <family val="2"/>
       </rPr>
-      <t>Book 1</t>
+      <t>Notes</t>
     </r>
     <r>
       <rPr>
@@ -444,16 +1755,16 @@
         <rFont val="Menlo"/>
         <family val="2"/>
       </rPr>
-      <t>https://probml.github.io/pml-book/book1.html</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF3B3B3B"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">): 10.1, 10.2.1, 10.2.3, 10.3.1-10.3.3 </t>
+      <t>../lecture3-logistic-regression/notes.qmd</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF3B3B3B"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>) [Slides](../lecture3-logistic-regression/filled-slides-pt2.qmd)</t>
     </r>
   </si>
   <si>
@@ -486,102 +1797,6 @@
         <rFont val="Menlo"/>
         <family val="2"/>
       </rPr>
-      <t>../lecture3-logistic-regression/notes.qmd</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF3B3B3B"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>)</t>
-    </r>
-  </si>
-  <si>
-    <t>Lecture 4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Multinomial logistic regression </t>
-  </si>
-  <si>
-    <t xml:space="preserve">[Book 1](https://probml.github.io/pml-book/book1.html): 10.2.2 </t>
-  </si>
-  <si>
-    <t>Feature transforms</t>
-  </si>
-  <si>
-    <r>
-      <t>[</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFA31515"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>Book 1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF3B3B3B"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>](</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="12"/>
-        <color rgb="FF3B3B3B"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>https://probml.github.io/pml-book/book1.html</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF3B3B3B"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>): 13.1, 13.2</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>[</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFA31515"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>Notes</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF3B3B3B"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>](</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="12"/>
-        <color rgb="FF3B3B3B"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
       <t>../lecture4-feature-transforms/notes.qmd</t>
     </r>
     <r>
@@ -591,1181 +1806,8 @@
         <rFont val="Menlo"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">) </t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Neural networks </t>
-  </si>
-  <si>
-    <r>
-      <t>[</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFA31515"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>Book 1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF3B3B3B"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>](</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="12"/>
-        <color rgb="FF3B3B3B"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>https://probml.github.io/pml-book/book1.html</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF3B3B3B"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">): 13.1, 13.2 </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>[</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFA31515"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>Notes</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF3B3B3B"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>](</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="12"/>
-        <color rgb="FF3B3B3B"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>../lecture5-neural-networks-intro/notes.qmd</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF3B3B3B"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">) </t>
-    </r>
-  </si>
-  <si>
-    <t>lecture 7</t>
-  </si>
-  <si>
-    <r>
-      <t>Homework 3 assigned ([</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFA31515"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>Drive</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF3B3B3B"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>](</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="12"/>
-        <color rgb="FF3B3B3B"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>https://drive.google.com/drive/folders/1Df96GdFpucM-YUf6c5PTWUfxWY-UrLXl?usp=drive_link</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF3B3B3B"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>))</t>
-    </r>
-  </si>
-  <si>
-    <t>Deep neural networks</t>
-  </si>
-  <si>
-    <t>Automatic Differentiation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[Book 1](https://probml.github.io/pml-book/book1.html): 13.3 </t>
-  </si>
-  <si>
-    <r>
-      <t>[</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFA31515"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>Notes</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF3B3B3B"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>](</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="12"/>
-        <color rgb="FF3B3B3B"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>../lecture6-backpropagation/notes.qmd</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF3B3B3B"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">) </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Homework 4 assigned ([</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFA31515"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>Drive</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF3B3B3B"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>](</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="12"/>
-        <color rgb="FF3B3B3B"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>https://drive.google.com/drive/folders/1wIblhOu4c0LlbiveKP1Z2uTVre3d62pO?usp=drive_link</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF3B3B3B"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>))</t>
-    </r>
-  </si>
-  <si>
-    <t>Homework 3 Due</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reverse-mode Automatic Differentiation </t>
-  </si>
-  <si>
-    <r>
-      <t>[</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFA31515"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>Book 1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF3B3B3B"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>](</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="12"/>
-        <color rgb="FF3B3B3B"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>https://probml.github.io/pml-book/book1.html</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF3B3B3B"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">): 13.4.5, 13.5 </t>
-    </r>
-  </si>
-  <si>
-    <t>PyTorch</t>
-  </si>
-  <si>
-    <r>
-      <t>[</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFA31515"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>Book 1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF3B3B3B"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>](</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="12"/>
-        <color rgb="FF3B3B3B"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>https://probml.github.io/pml-book/book1.html</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF3B3B3B"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>): 13.5</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve"> [Notebook](https://drive.google.com/file/d/1N76hpENuKchbfN0o-NZ02FAgZYPiWPVf/view?usp=drive_link)</t>
-  </si>
-  <si>
-    <r>
-      <t>Homework 5 assigned ([</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFA31515"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>Drive</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF3B3B3B"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>](</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="12"/>
-        <color rgb="FF3B3B3B"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>https://drive.google.com/drive/folders/1C9vFAnO_sogGupxvOrU4uQl8ZkF7seU5?usp=drive_link</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF3B3B3B"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>))</t>
-    </r>
-  </si>
-  <si>
-    <t>Homework 4 Due</t>
-  </si>
-  <si>
-    <t xml:space="preserve">L1 &amp; L2 regularization </t>
-  </si>
-  <si>
-    <r>
-      <t>[</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFA31515"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>Book 1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF3B3B3B"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>](</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="12"/>
-        <color rgb="FF3B3B3B"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>https://probml.github.io/pml-book/book1.html</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF3B3B3B"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">): 8.4 </t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Regularization (Cont.), Dropout </t>
-  </si>
-  <si>
-    <r>
-      <t>[</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFA31515"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>Book 1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF3B3B3B"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>](</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="12"/>
-        <color rgb="FF3B3B3B"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>https://probml.github.io/pml-book/book1.html</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF3B3B3B"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>): 13.4.1-13.4.2</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Homework 6 assigned ([</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFA31515"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>Drive</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF3B3B3B"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>](</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="12"/>
-        <color rgb="FF3B3B3B"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>https://drive.google.com/drive/u/1/folders/1ohI5itSgEhBNmKSLQSjwmJlgWjioWDhi</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF3B3B3B"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>))</t>
-    </r>
-  </si>
-  <si>
-    <t>Homework 5 Due</t>
-  </si>
-  <si>
-    <t>Stochastic gradient descent</t>
-  </si>
-  <si>
-    <r>
-      <t>[</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFA31515"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>Book 1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF3B3B3B"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>](</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="12"/>
-        <color rgb="FF3B3B3B"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>https://probml.github.io/pml-book/book1.html</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF3B3B3B"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">): 14.1-14.3 </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>[</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFA31515"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>Notes</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF3B3B3B"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>](</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="12"/>
-        <color rgb="FF3B3B3B"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>../lecture9-optimization/notes.qmd</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF3B3B3B"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">) </t>
-    </r>
-  </si>
-  <si>
-    <t>Homework 6 Due</t>
-  </si>
-  <si>
-    <t>Spring break</t>
-  </si>
-  <si>
-    <t>Project Proposal Due</t>
-  </si>
-  <si>
-    <t>Residual networks and Normalization</t>
-  </si>
-  <si>
-    <t>Residual networks and Normalization (cont.)</t>
-  </si>
-  <si>
-    <r>
-      <t>[</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFA31515"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>Book 1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF3B3B3B"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>](</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="12"/>
-        <color rgb="FF3B3B3B"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>https://probml.github.io/pml-book/book1.html</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF3B3B3B"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">): 15.1, 15.2.1-15.2.3 </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>[</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFA31515"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>Slides</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF3B3B3B"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>](</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="12"/>
-        <color rgb="FF3B3B3B"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>./notes/lecture14.pdf</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF3B3B3B"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">) </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>[</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFA31515"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>Slides</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF3B3B3B"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>](</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="12"/>
-        <color rgb="FF3B3B3B"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>./notes/lecture15.pdf</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF3B3B3B"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">) </t>
-    </r>
-  </si>
-  <si>
-    <t>Convolutional Networks</t>
-  </si>
-  <si>
-    <t>Convolutional Networks (cont.)</t>
-  </si>
-  <si>
-    <r>
-      <t>[</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFA31515"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>Slides</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF3B3B3B"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>](</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="12"/>
-        <color rgb="FF3B3B3B"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>./notes/lecture16.pdf</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF3B3B3B"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">) </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>[</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFA31515"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>Book 1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF3B3B3B"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>](</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="12"/>
-        <color rgb="FF3B3B3B"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>https://probml.github.io/pml-book/book1.html</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF3B3B3B"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">): 15.2.5-15.2.7 </t>
-    </r>
-  </si>
-  <si>
-    <t>Language models, RNNs</t>
-  </si>
-  <si>
-    <r>
-      <t>Homework 7 assigned ([</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFA31515"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>Drive</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF3B3B3B"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>](</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="12"/>
-        <color rgb="FF3B3B3B"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>https://drive.google.com/drive/folders/1vZYEOfmDCfGxWMAAXeEwgMlvCOfKUgle?usp=drive_link</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF3B3B3B"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>))</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Homework 8 assigned ([</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFA31515"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>Drive</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF3B3B3B"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>](</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="12"/>
-        <color rgb="FF3B3B3B"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>https://drive.google.com/drive/folders/1lO11Br_irrOckxZVZdi72MSjR8lTvQ_O?usp=drive_link</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF3B3B3B"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>))</t>
-    </r>
-  </si>
-  <si>
-    <t>[Book 1](https://probml.github.io/pml-book/book1.html): 15.2.1-15.2.6</t>
-  </si>
-  <si>
-    <r>
-      <t>[</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFA31515"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>Slides</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF3B3B3B"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>](</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="12"/>
-        <color rgb="FF3B3B3B"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>./notes/lecture17.pdf</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF3B3B3B"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">) </t>
-    </r>
-  </si>
-  <si>
-    <t>Autoencoders &amp; U-Nets</t>
-  </si>
-  <si>
-    <t>Image models</t>
-  </si>
-  <si>
-    <t>Homework 7 Due</t>
-  </si>
-  <si>
-    <t>Homework 9 assigned</t>
-  </si>
-  <si>
-    <t>Homework 8 Due</t>
-  </si>
-  <si>
-    <r>
-      <t>[</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFA31515"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>Book 1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF3B3B3B"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>](</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="12"/>
-        <color rgb="FF3B3B3B"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>https://probml.github.io/pml-book/book1.html</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF3B3B3B"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>): 15.2.1-15.2.6</t>
-    </r>
-  </si>
-  <si>
-    <t>Attention layers</t>
-  </si>
-  <si>
-    <t>Homework 10 assigned</t>
-  </si>
-  <si>
-    <t>Project check-in assigned</t>
-  </si>
-  <si>
-    <t>Homework 9 Due</t>
-  </si>
-  <si>
-    <t>Transformers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Transformers (cont.), Large language models </t>
-  </si>
-  <si>
-    <t>Lecture 25</t>
-  </si>
-  <si>
-    <t>Project check-in due</t>
-  </si>
-  <si>
-    <t>Addressing bias in machine learning</t>
-  </si>
-  <si>
-    <t>Impacts of machine learning</t>
-  </si>
-  <si>
-    <t>Homework 10 Due</t>
-  </si>
-  <si>
-    <t>[Assignment](../assignments/homeworks/homeworks.qmd#Homework-1)</t>
-  </si>
-  <si>
-    <t>[Assignment](../assignments/homeworks/homeworks.qmd#Homework-2)</t>
-  </si>
-  <si>
-    <t>[Assignment](../assignments/homeworks/homeworks.qmd#Homework-3)</t>
-  </si>
-  <si>
-    <t>[Assignment](../assignments/homeworks/homeworks.qmd#Homework-4)</t>
-  </si>
-  <si>
-    <t>[Assignment](../assignments/homeworks/homeworks.qmd#Homework-5)</t>
-  </si>
-  <si>
-    <t>[Assignment](../assignments/homeworks/homeworks.qmd#Homework-6)</t>
-  </si>
-  <si>
-    <t>[Assignment](../assignments/homeworks/homeworks.qmd#Homework-7)</t>
-  </si>
-  <si>
-    <t>[Assignment](../assignments/homeworks/homeworks.qmd#Homework-8)</t>
-  </si>
-  <si>
-    <t>[Assignment](../assignments/homeworks/homeworks.qmd#Homework-9)</t>
-  </si>
-  <si>
-    <t>[Assignment](../assignments/homeworks/homeworks.qmd#Homework-10)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Final project ethics warm-up assigned </t>
-  </si>
-  <si>
-    <t>Ethics Warm-up Due</t>
-  </si>
-  <si>
-    <t>[Assignment](../assignments/final-project/ethics.qmd)</t>
-  </si>
-  <si>
-    <t>[Assignment](../assignments/final-project/outline.qmd)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[Prerequisites](../lecture1-background/prereqs.qmd) [Notes](../lecture1-background/notes.qmd) [slides](../lecture1-background/slides.pdf) </t>
-  </si>
-  <si>
-    <r>
-      <t>[</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFA31515"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>Notes</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF3B3B3B"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>](</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="12"/>
-        <color rgb="FF3B3B3B"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>../lecture8-regularization/notes.qmd</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF3B3B3B"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>[</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFA31515"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>Notes</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF3B3B3B"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>](</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="12"/>
-        <color rgb="FF3B3B3B"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>../lecture8-regularization/notes.qmd</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF3B3B3B"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">) </t>
-    </r>
-  </si>
-  <si>
-    <t>[Notes](../lecture2-linear-regression/notes.qmd) [Blank slides](../lecture2-linear-regression/slides.pdf)</t>
+      <t xml:space="preserve">) [Slides](../lecture4-feature-transforms/filled-slides.pdf)  [Blank](../lecture4-feature-transforms/slides.pdf) </t>
+    </r>
   </si>
 </sst>
 </file>
@@ -3014,7 +3056,7 @@
   <dimension ref="A1:H45"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="75" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="48" customHeight="1"/>
@@ -3088,7 +3130,7 @@
         <v>54</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>55</v>
@@ -3114,7 +3156,7 @@
         <v>59</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>60</v>
@@ -3137,13 +3179,13 @@
         <v>59</v>
       </c>
       <c r="F5" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="G5" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="H5" s="8" t="s">
         <v>63</v>
-      </c>
-      <c r="H5" s="8" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="48" customHeight="1">
@@ -3159,7 +3201,7 @@
       <c r="D6" s="8"/>
       <c r="E6" s="8"/>
       <c r="F6" s="8" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>18</v>
@@ -3176,16 +3218,16 @@
         <v>8</v>
       </c>
       <c r="D7" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="E7" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="E7" s="8" t="s">
+      <c r="F7" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="G7" s="2" t="s">
         <v>66</v>
-      </c>
-      <c r="F7" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="48" customHeight="1">
@@ -3199,19 +3241,19 @@
         <v>8</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>67</v>
+        <v>152</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>13</v>
       </c>
       <c r="H8" s="8" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="48" customHeight="1">
@@ -3227,7 +3269,7 @@
       <c r="D9" s="8"/>
       <c r="E9" s="5"/>
       <c r="F9" s="8" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>51</v>
@@ -3245,13 +3287,13 @@
         <v>8</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>73</v>
+        <v>153</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>14</v>
@@ -3268,19 +3310,19 @@
         <v>8</v>
       </c>
       <c r="D11" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="G11" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="E11" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="F11" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>77</v>
-      </c>
       <c r="H11" s="8" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="48" customHeight="1">
@@ -3296,10 +3338,10 @@
       <c r="D12" s="2"/>
       <c r="E12" s="5"/>
       <c r="F12" s="8" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="48" customHeight="1">
@@ -3313,13 +3355,13 @@
         <v>8</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>16</v>
@@ -3336,19 +3378,19 @@
         <v>8</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>20</v>
       </c>
       <c r="H14" s="8" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="48" customHeight="1">
@@ -3364,10 +3406,10 @@
       <c r="D15" s="8"/>
       <c r="E15" s="5"/>
       <c r="F15" s="8" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="48" customHeight="1">
@@ -3381,13 +3423,13 @@
         <v>8</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="G16" s="2" t="s">
         <v>21</v>
@@ -3404,19 +3446,19 @@
         <v>8</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="G17" s="2" t="s">
         <v>23</v>
       </c>
       <c r="H17" s="8" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="48" customHeight="1">
@@ -3432,10 +3474,10 @@
       <c r="D18" s="8"/>
       <c r="E18" s="8"/>
       <c r="F18" s="8" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="H18" s="8"/>
     </row>
@@ -3450,13 +3492,13 @@
         <v>8</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="G19" s="2" t="s">
         <v>25</v>
@@ -3473,19 +3515,19 @@
         <v>8</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="G20" s="2" t="s">
         <v>26</v>
       </c>
       <c r="H20" s="8" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="48" customHeight="1">
@@ -3501,10 +3543,10 @@
       <c r="D21" s="8"/>
       <c r="E21" s="8"/>
       <c r="F21" s="8" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="H21" s="8"/>
     </row>
@@ -3519,13 +3561,13 @@
         <v>8</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="F22" s="8" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="G22" s="2" t="s">
         <v>28</v>
@@ -3542,13 +3584,13 @@
         <v>8</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="F23" s="8" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="G23" s="2" t="s">
         <v>29</v>
@@ -3567,10 +3609,10 @@
       <c r="D24" s="2"/>
       <c r="E24" s="5"/>
       <c r="F24" s="8" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="48" customHeight="1">
@@ -3587,7 +3629,7 @@
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
       <c r="G25" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="48" customHeight="1">
@@ -3601,13 +3643,13 @@
         <v>8</v>
       </c>
       <c r="D26" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="E26" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="F26" s="8" t="s">
         <v>104</v>
-      </c>
-      <c r="E26" s="8" t="s">
-        <v>106</v>
-      </c>
-      <c r="F26" s="8" t="s">
-        <v>107</v>
       </c>
       <c r="G26" s="2" t="s">
         <v>31</v>
@@ -3624,13 +3666,13 @@
         <v>8</v>
       </c>
       <c r="D27" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="E27" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="F27" s="8" t="s">
         <v>105</v>
-      </c>
-      <c r="E27" s="8" t="s">
-        <v>106</v>
-      </c>
-      <c r="F27" s="8" t="s">
-        <v>108</v>
       </c>
       <c r="G27" s="2" t="s">
         <v>32</v>
@@ -3649,10 +3691,10 @@
       <c r="D28" s="2"/>
       <c r="E28" s="5"/>
       <c r="F28" s="5" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="48" customHeight="1">
@@ -3666,13 +3708,13 @@
         <v>8</v>
       </c>
       <c r="D29" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="E29" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="E29" s="8" t="s">
-        <v>112</v>
-      </c>
       <c r="F29" s="8" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="G29" s="2" t="s">
         <v>34</v>
@@ -3689,19 +3731,19 @@
         <v>8</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="E30" s="8" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="F30" s="8" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="G30" s="2" t="s">
         <v>35</v>
       </c>
       <c r="H30" s="8" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="48" customHeight="1">
@@ -3717,10 +3759,10 @@
       <c r="D31" s="8"/>
       <c r="E31" s="8"/>
       <c r="F31" s="8" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="H31" s="8"/>
     </row>
@@ -3735,10 +3777,10 @@
         <v>8</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="F32" s="8"/>
       <c r="G32" s="2" t="s">
@@ -3756,7 +3798,7 @@
         <v>8</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="E33" s="5"/>
       <c r="F33" s="7"/>
@@ -3764,7 +3806,7 @@
         <v>38</v>
       </c>
       <c r="H33" s="10" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="34" spans="1:8" ht="48" customHeight="1">
@@ -3780,10 +3822,10 @@
       <c r="D34" s="2"/>
       <c r="E34" s="5"/>
       <c r="F34" s="1" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="G34" s="8" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="H34" s="10"/>
     </row>
@@ -3798,13 +3840,13 @@
         <v>8</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="E35" s="8" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="F35" s="8" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="G35" s="2" t="s">
         <v>40</v>
@@ -3821,7 +3863,7 @@
         <v>8</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E36" s="5"/>
       <c r="F36" s="5"/>
@@ -3829,7 +3871,7 @@
         <v>41</v>
       </c>
       <c r="H36" s="9" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="48" customHeight="1">
@@ -3845,10 +3887,10 @@
       <c r="D37" s="2"/>
       <c r="E37" s="5"/>
       <c r="F37" s="8" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="38" spans="1:8" ht="48" customHeight="1">
@@ -3862,7 +3904,7 @@
         <v>8</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="E38" s="5"/>
       <c r="F38" s="5"/>
@@ -3881,15 +3923,15 @@
         <v>8</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="E39" s="5"/>
       <c r="F39" s="5"/>
       <c r="G39" s="2" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="H39" s="9" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="40" spans="1:8" ht="48" customHeight="1">
@@ -3905,10 +3947,10 @@
       <c r="D40" s="2"/>
       <c r="E40" s="5"/>
       <c r="F40" s="1" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="41" spans="1:8" ht="48" customHeight="1">
@@ -3922,7 +3964,7 @@
         <v>8</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="E41" s="5"/>
       <c r="F41" s="5"/>
@@ -3941,7 +3983,7 @@
         <v>8</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="E42" s="5"/>
       <c r="F42" s="5"/>
@@ -3962,10 +4004,10 @@
       <c r="D43" s="2"/>
       <c r="E43" s="5"/>
       <c r="F43" s="8" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="44" spans="1:8" ht="48" customHeight="1">
@@ -3981,7 +4023,7 @@
       <c r="D44" s="5"/>
       <c r="E44" s="5"/>
       <c r="F44" s="1" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="G44" s="2" t="s">
         <v>49</v>
@@ -4004,7 +4046,7 @@
         <v>50</v>
       </c>
       <c r="H45" s="8" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
   </sheetData>

</xml_diff>